<commit_message>
Updated dbCAN - Prop CAZymes from ORFs
</commit_message>
<xml_diff>
--- a/dbcan/prodigalCounts.xlsx
+++ b/dbcan/prodigalCounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/OG_MetaG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/OG_MetaG/dbcan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{DC09E487-9377-4218-8BD1-DE609723599B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C6339950-622D-4D31-B08C-16BBD1934450}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{DC09E487-9377-4218-8BD1-DE609723599B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2C155171-C756-4C94-B1D9-D0AE0CA249E7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A54C7707-2D3C-4C30-9A53-F95EF17DF46D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A54C7707-2D3C-4C30-9A53-F95EF17DF46D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Total ORFs</t>
   </si>
@@ -43,18 +43,6 @@
   </si>
   <si>
     <t>% CAZyme from ORFs</t>
-  </si>
-  <si>
-    <t>Season</t>
-  </si>
-  <si>
-    <t>Summer</t>
-  </si>
-  <si>
-    <t>Winter</t>
-  </si>
-  <si>
-    <t>Spring</t>
   </si>
 </sst>
 </file>
@@ -406,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519A3502-1BAD-42F0-AF29-BFABB4C61DF6}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,77 +498,45 @@
         <v>19489</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <f>B3/B2</f>
-        <v>3.8378990208873247E-2</v>
+        <f>(B3/B2)*100</f>
+        <v>3.8378990208873245</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:J4" si="0">C3/C2</f>
-        <v>2.0642018930540986E-2</v>
+        <f t="shared" ref="C4:J4" si="0">(C3/C2)*100</f>
+        <v>2.0642018930540984</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>3.9271011610157731E-2</v>
+        <v>3.9271011610157731</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>3.8510920254400886E-2</v>
+        <v>3.8510920254400887</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>3.8264366570979799E-2</v>
+        <v>3.8264366570979798</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>4.3215377410871121E-2</v>
+        <v>4.3215377410871119</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>3.6567677578398211E-2</v>
+        <v>3.656767757839821</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>3.5314716866430361E-2</v>
+        <v>3.531471686643036</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>3.8102555680680682E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>6</v>
+        <v>3.8102555680680683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>